<commit_message>
updated + finished work
</commit_message>
<xml_diff>
--- a/assignments/week2 assignment-1.xlsx
+++ b/assignments/week2 assignment-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2022fall\TA\22fall\week2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Humna\Documents\GitHub\mis201\assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB9DBA2-3C05-41B6-A7B3-74FE3C005F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CAB018-429C-469E-A330-EFCBEE5CD27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5618BDF1-8B4C-43A4-97B2-C519E045C55F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{5618BDF1-8B4C-43A4-97B2-C519E045C55F}"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="2" r:id="rId1"/>
@@ -26,9 +26,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="134">
   <si>
     <t>customer_number</t>
   </si>
@@ -366,6 +367,78 @@
   </si>
   <si>
     <t>the stree name in the stree_address</t>
+  </si>
+  <si>
+    <t>Conan Adiscot</t>
+  </si>
+  <si>
+    <t>Darya D'Alessandro</t>
+  </si>
+  <si>
+    <t>Griz Hardaker</t>
+  </si>
+  <si>
+    <t>Joete Rainsden</t>
+  </si>
+  <si>
+    <t>Pate Frew</t>
+  </si>
+  <si>
+    <t>Marla Buckley</t>
+  </si>
+  <si>
+    <t>Lorain Howroyd</t>
+  </si>
+  <si>
+    <t>Chiquita Spires</t>
+  </si>
+  <si>
+    <t>Yves Carlyon</t>
+  </si>
+  <si>
+    <t>Elsinore Strangman</t>
+  </si>
+  <si>
+    <t>Spenser Crosston</t>
+  </si>
+  <si>
+    <t>Lucien Bordes</t>
+  </si>
+  <si>
+    <t>Maple Place</t>
+  </si>
+  <si>
+    <t>Hanson Center</t>
+  </si>
+  <si>
+    <t>Memorial Junction</t>
+  </si>
+  <si>
+    <t>Norway Maple Junction</t>
+  </si>
+  <si>
+    <t>Laurel Court</t>
+  </si>
+  <si>
+    <t>Knutson Terrace</t>
+  </si>
+  <si>
+    <t>Bashford Way</t>
+  </si>
+  <si>
+    <t>Troy Trail</t>
+  </si>
+  <si>
+    <t>Arkansas Pass</t>
+  </si>
+  <si>
+    <t>Lillian Road</t>
+  </si>
+  <si>
+    <t>Toban Center</t>
+  </si>
+  <si>
+    <t>Thackeray Junction</t>
   </si>
 </sst>
 </file>
@@ -855,16 +928,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2F30A7-4CB3-4B67-8058-5CD40E902587}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="4" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="29.90625" customWidth="1"/>
+    <col min="3" max="4" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>104</v>
       </c>
@@ -881,7 +956,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>96</v>
       </c>
@@ -895,7 +970,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -905,9 +980,12 @@
       <c r="C3" s="1">
         <v>569</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D3" s="1">
+        <f>B3-C3</f>
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -917,9 +995,12 @@
       <c r="C4" s="1">
         <v>1402</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D11" si="0">B4-C4</f>
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -929,9 +1010,12 @@
       <c r="C5" s="1">
         <v>1237</v>
       </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -941,9 +1025,12 @@
       <c r="C6" s="1">
         <v>650</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>2875</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -953,9 +1040,12 @@
       <c r="C7" s="1">
         <v>650</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>616</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -965,9 +1055,12 @@
       <c r="C8" s="1">
         <v>1017</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>4640</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -977,9 +1070,12 @@
       <c r="C9" s="1">
         <v>532</v>
       </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -989,9 +1085,12 @@
       <c r="C10" s="1">
         <v>1115</v>
       </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>861</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1001,7 +1100,10 @@
       <c r="C11" s="1">
         <v>506</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>728</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1012,17 +1114,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0417C0CF-604D-4365-B01F-DD8BBE550231}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6328125" customWidth="1"/>
+    <col min="2" max="2" width="33.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>105</v>
       </c>
@@ -1035,7 +1137,7 @@
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
     </row>
-    <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>85</v>
       </c>
@@ -1061,7 +1163,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>86</v>
       </c>
@@ -1087,19 +1189,40 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="8">
+        <f>100-B3</f>
+        <v>65</v>
+      </c>
+      <c r="C4" s="8">
+        <f t="shared" ref="C4:H4" si="0">100-C3</f>
+        <v>71</v>
+      </c>
+      <c r="D4" s="8">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>88</v>
       </c>
@@ -1107,7 +1230,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>106</v>
       </c>
@@ -1128,7 +1251,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
     </row>
-    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>100</v>
       </c>
@@ -1149,7 +1272,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="13"/>
       <c r="C10" s="19" t="s">
@@ -1170,7 +1293,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
     </row>
-    <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>96</v>
       </c>
@@ -1193,106 +1316,259 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>2003</v>
+      </c>
+      <c r="C12" s="8">
+        <f>B12*(1-B23)</f>
+        <v>1802.7</v>
+      </c>
+      <c r="D12" s="8">
+        <f>B12*(1-C23)</f>
+        <v>1702.55</v>
+      </c>
+      <c r="E12" s="8">
+        <f>B12*(1-D23)</f>
+        <v>1602.4</v>
+      </c>
+      <c r="F12" s="8">
+        <f>B12*(1-E23)</f>
+        <v>1662.49</v>
+      </c>
+      <c r="G12" s="8">
+        <f>B12*(1-F23)</f>
+        <v>1742.61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>2</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>3511</v>
+      </c>
+      <c r="C13" s="8">
+        <f>B13*(1-B23)</f>
+        <v>3159.9</v>
+      </c>
+      <c r="D13" s="8">
+        <f>B13*(1-C23)</f>
+        <v>2984.35</v>
+      </c>
+      <c r="E13" s="8">
+        <f>B13*(1-D23)</f>
+        <v>2808.8</v>
+      </c>
+      <c r="F13" s="8">
+        <f>B13*(1-E23)</f>
+        <v>2914.1299999999997</v>
+      </c>
+      <c r="G13" s="8">
+        <f>B13*(1-F23)</f>
+        <v>3054.57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>3</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>2462</v>
+      </c>
+      <c r="C14" s="8">
+        <f>B14*(1-B23)</f>
+        <v>2215.8000000000002</v>
+      </c>
+      <c r="D14" s="8">
+        <f>B14*(1-C23)</f>
+        <v>2092.6999999999998</v>
+      </c>
+      <c r="E14" s="8">
+        <f>B14*(1-D23)</f>
+        <v>1969.6000000000001</v>
+      </c>
+      <c r="F14" s="8">
+        <f>B14*(1-E23)</f>
+        <v>2043.4599999999998</v>
+      </c>
+      <c r="G14" s="8">
+        <f>B14*(1-F23)</f>
+        <v>2141.94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>4</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>3525</v>
+      </c>
+      <c r="C15" s="8">
+        <f>B15*(1-B23)</f>
+        <v>3172.5</v>
+      </c>
+      <c r="D15" s="8">
+        <f>B15*(1-C23)</f>
+        <v>2996.25</v>
+      </c>
+      <c r="E15" s="8">
+        <f>B15*(1-D23)</f>
+        <v>2820</v>
+      </c>
+      <c r="F15" s="8">
+        <f>B15*(1-E23)</f>
+        <v>2925.75</v>
+      </c>
+      <c r="G15" s="8">
+        <f>B15*(1-F23)</f>
+        <v>3066.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>5</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>1266</v>
+      </c>
+      <c r="C16" s="8">
+        <f>B16*(1-B23)</f>
+        <v>1139.4000000000001</v>
+      </c>
+      <c r="D16" s="8">
+        <f>B16*(1-C23)</f>
+        <v>1076.0999999999999</v>
+      </c>
+      <c r="E16" s="8">
+        <f>B16*(1-D23)</f>
+        <v>1012.8000000000001</v>
+      </c>
+      <c r="F16" s="8">
+        <f>B16*(1-E23)</f>
+        <v>1050.78</v>
+      </c>
+      <c r="G16" s="8">
+        <f>B16*(1-F23)</f>
+        <v>1101.42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>6</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>5657</v>
+      </c>
+      <c r="C17" s="8">
+        <f>B17*(1-B23)</f>
+        <v>5091.3</v>
+      </c>
+      <c r="D17" s="8">
+        <f>B17*(1-C23)</f>
+        <v>4808.45</v>
+      </c>
+      <c r="E17" s="8">
+        <f>B17*(1-D23)</f>
+        <v>4525.6000000000004</v>
+      </c>
+      <c r="F17" s="8">
+        <f>B17*(1-E23)</f>
+        <v>4695.3099999999995</v>
+      </c>
+      <c r="G17" s="8">
+        <f>B17*(1-F23)</f>
+        <v>4921.59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>7</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>2357</v>
+      </c>
+      <c r="C18" s="8">
+        <f>B18*(1-B23)</f>
+        <v>2121.3000000000002</v>
+      </c>
+      <c r="D18" s="8">
+        <f>B18*(1-C23)</f>
+        <v>2003.45</v>
+      </c>
+      <c r="E18" s="8">
+        <f>B18*(1-D23)</f>
+        <v>1885.6000000000001</v>
+      </c>
+      <c r="F18" s="8">
+        <f>B18*(1-E23)</f>
+        <v>1956.31</v>
+      </c>
+      <c r="G18" s="8">
+        <f>B18*(1-F23)</f>
+        <v>2050.59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>8</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>1976</v>
+      </c>
+      <c r="C19" s="8">
+        <f>B19*(1-B23)</f>
+        <v>1778.4</v>
+      </c>
+      <c r="D19" s="8">
+        <f>B19*(1-C23)</f>
+        <v>1679.6</v>
+      </c>
+      <c r="E19" s="8">
+        <f>B19*(1-D23)</f>
+        <v>1580.8000000000002</v>
+      </c>
+      <c r="F19" s="8">
+        <f>B19*(1-E23)</f>
+        <v>1640.08</v>
+      </c>
+      <c r="G19" s="8">
+        <f>B19*(1-F23)</f>
+        <v>1719.12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>9</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <v>1234</v>
+      </c>
+      <c r="C20" s="8">
+        <f>B20*(1-B23)</f>
+        <v>1110.6000000000001</v>
+      </c>
+      <c r="D20" s="8">
+        <f>B20*(1-C23)</f>
+        <v>1048.8999999999999</v>
+      </c>
+      <c r="E20" s="8">
+        <f>B20*(1-D23)</f>
+        <v>987.2</v>
+      </c>
+      <c r="F20" s="8">
+        <f>B20*(1-E23)</f>
+        <v>1024.22</v>
+      </c>
+      <c r="G20" s="8">
+        <f>B20*(1-E23)</f>
+        <v>1024.22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>98</v>
       </c>
@@ -1312,7 +1588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>97</v>
       </c>
@@ -1345,24 +1621,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4636BD3-2698-49F0-84AB-8C4707E75367}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>107</v>
       </c>
@@ -1377,7 +1653,7 @@
       <c r="J1" s="20"/>
       <c r="L1" s="15"/>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1682,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1435,7 +1711,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1457,9 +1733,14 @@
       <c r="G4" s="1">
         <v>80299</v>
       </c>
-      <c r="L4" s="15"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K4" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -1481,9 +1762,14 @@
       <c r="G5" s="1">
         <v>17622</v>
       </c>
-      <c r="L5" s="15"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K5" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1505,9 +1791,14 @@
       <c r="G6" s="1">
         <v>46216</v>
       </c>
-      <c r="L6" s="15"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1529,9 +1820,14 @@
       <c r="G7" s="1">
         <v>46216</v>
       </c>
-      <c r="L7" s="15"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K7" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1553,9 +1849,14 @@
       <c r="G8" s="1">
         <v>55172</v>
       </c>
-      <c r="L8" s="15"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K8" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -1577,9 +1878,14 @@
       <c r="G9" s="1">
         <v>46216</v>
       </c>
-      <c r="L9" s="15"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K9" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -1601,9 +1907,14 @@
       <c r="G10" s="1">
         <v>93381</v>
       </c>
-      <c r="L10" s="15"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K10" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
@@ -1625,9 +1936,14 @@
       <c r="G11" s="1">
         <v>79934</v>
       </c>
-      <c r="L11" s="15"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -1649,9 +1965,14 @@
       <c r="G12" s="1">
         <v>79934</v>
       </c>
-      <c r="L12" s="15"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -1673,9 +1994,14 @@
       <c r="G13" s="1">
         <v>78703</v>
       </c>
-      <c r="L13" s="15"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K13" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>54</v>
       </c>
@@ -1697,9 +2023,14 @@
       <c r="G14" s="1">
         <v>32230</v>
       </c>
-      <c r="L14" s="15"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K14" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>60</v>
       </c>
@@ -1721,9 +2052,14 @@
       <c r="G15" s="1">
         <v>21282</v>
       </c>
-      <c r="L15" s="15"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K15" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>60</v>
       </c>
@@ -1745,9 +2081,14 @@
       <c r="G16" s="1">
         <v>21282</v>
       </c>
-      <c r="L16" s="15"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K16" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>60</v>
       </c>
@@ -1769,9 +2110,14 @@
       <c r="G17" s="1">
         <v>21282</v>
       </c>
-      <c r="L17" s="15"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K17" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="L17" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>66</v>
       </c>
@@ -1793,9 +2139,14 @@
       <c r="G18" s="1">
         <v>70820</v>
       </c>
-      <c r="L18" s="15"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K18" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>72</v>
       </c>
@@ -1817,9 +2168,14 @@
       <c r="G19" s="1">
         <v>95219</v>
       </c>
-      <c r="L19" s="15"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K19" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>77</v>
       </c>
@@ -1841,9 +2197,14 @@
       <c r="G20" s="1">
         <v>32309</v>
       </c>
-      <c r="L20" s="15"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K20" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>77</v>
       </c>
@@ -1865,7 +2226,12 @@
       <c r="G21" s="1">
         <v>32309</v>
       </c>
-      <c r="L21" s="15"/>
+      <c r="K21" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1880,22 +2246,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7F6382-8D3B-4AC1-996E-845AF37E0BB8}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1927,7 +2294,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1950,7 +2317,7 @@
         <v>20566</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1973,7 +2340,7 @@
         <v>80299</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1996,7 +2363,7 @@
         <v>17622</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -2019,7 +2386,7 @@
         <v>46216</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -2042,7 +2409,7 @@
         <v>46216</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
@@ -2065,7 +2432,7 @@
         <v>55172</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2088,7 +2455,7 @@
         <v>46216</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
@@ -2111,7 +2478,7 @@
         <v>93381</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -2134,7 +2501,7 @@
         <v>79934</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
@@ -2157,7 +2524,7 @@
         <v>79934</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
@@ -2180,7 +2547,7 @@
         <v>78703</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>54</v>
       </c>
@@ -2203,7 +2570,7 @@
         <v>32230</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
@@ -2226,7 +2593,7 @@
         <v>21282</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>60</v>
       </c>
@@ -2249,7 +2616,7 @@
         <v>21282</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>60</v>
       </c>
@@ -2272,7 +2639,7 @@
         <v>21282</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
@@ -2295,7 +2662,7 @@
         <v>70820</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>72</v>
       </c>
@@ -2318,7 +2685,7 @@
         <v>95219</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>77</v>
       </c>
@@ -2341,7 +2708,7 @@
         <v>32309</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>77</v>
       </c>

</xml_diff>